<commit_message>
feat: initialize project with xlsx and papaparse dependencies
- Added xlsxworker.js for handling XLSX file processing in web workers.
- Created package.json to manage project metadata and dependencies.
- Generated package-lock.json to lock dependency versions.
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://azacessorios-my.sharepoint.com/personal/marcos_azacessorios_com_br/Documents/Documents/PythonStudy/MPRSeparator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_2B59D2BFD320D55BAFB82311595E10325E05FDC2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C120321-128B-4108-9318-5CBA740821BE}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_2B59D2BFD320D55BAFB82311595E10325E05FDC2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA68020-1060-4B18-9C51-934EBC5CA86E}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>OrderNumber</t>
   </si>
@@ -95,13 +95,73 @@
   </si>
   <si>
     <t xml:space="preserve">False </t>
+  </si>
+  <si>
+    <t>delete01</t>
+  </si>
+  <si>
+    <t>delete02</t>
+  </si>
+  <si>
+    <t>delete03</t>
+  </si>
+  <si>
+    <t>delete04</t>
+  </si>
+  <si>
+    <t>delete05</t>
+  </si>
+  <si>
+    <t>delete06</t>
+  </si>
+  <si>
+    <t>delete07</t>
+  </si>
+  <si>
+    <t>delete08</t>
+  </si>
+  <si>
+    <t>delete09</t>
+  </si>
+  <si>
+    <t>delete10</t>
+  </si>
+  <si>
+    <t>delete11</t>
+  </si>
+  <si>
+    <t>delete12</t>
+  </si>
+  <si>
+    <t>delete13</t>
+  </si>
+  <si>
+    <t>delete14</t>
+  </si>
+  <si>
+    <t>delete15</t>
+  </si>
+  <si>
+    <t>delete16</t>
+  </si>
+  <si>
+    <t>delete17</t>
+  </si>
+  <si>
+    <t>delete18</t>
+  </si>
+  <si>
+    <t>delete19</t>
+  </si>
+  <si>
+    <t>delete20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +173,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -461,7 +527,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,8 +553,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>100001</v>
+      <c r="A2" t="s">
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -501,8 +567,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100002</v>
+      <c r="A3" t="s">
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -515,8 +581,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>100003</v>
+      <c r="A4" t="s">
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -529,8 +595,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>100004</v>
+      <c r="A5" t="s">
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -543,8 +609,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>100005</v>
+      <c r="A6" t="s">
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -557,8 +623,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>100006</v>
+      <c r="A7" t="s">
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -571,8 +637,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>100007</v>
+      <c r="A8" t="s">
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -585,8 +651,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>100008</v>
+      <c r="A9" t="s">
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -599,8 +665,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>100009</v>
+      <c r="A10" t="s">
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -613,8 +679,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>100010</v>
+      <c r="A11" t="s">
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -627,8 +693,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>100011</v>
+      <c r="A12" t="s">
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -641,8 +707,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>100012</v>
+      <c r="A13" t="s">
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -655,8 +721,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>100013</v>
+      <c r="A14" t="s">
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -669,8 +735,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>100014</v>
+      <c r="A15" t="s">
+        <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -683,8 +749,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>100015</v>
+      <c r="A16" t="s">
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -697,8 +763,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>100016</v>
+      <c r="A17" t="s">
+        <v>40</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -711,8 +777,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>100017</v>
+      <c r="A18" t="s">
+        <v>41</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -725,8 +791,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>100018</v>
+      <c r="A19" t="s">
+        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
@@ -739,8 +805,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>100019</v>
+      <c r="A20" t="s">
+        <v>43</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -753,8 +819,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>100020</v>
+      <c r="A21" t="s">
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
@@ -767,6 +833,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>